<commit_message>
tambahan catatan revisi sipepeng
</commit_message>
<xml_diff>
--- a/DOKUMEN  PENDUKUNG/CATATAN REVISI.xlsx
+++ b/DOKUMEN  PENDUKUNG/CATATAN REVISI.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
   <si>
     <t xml:space="preserve">Print out / Laporan </t>
   </si>
@@ -178,6 +178,30 @@
   </si>
   <si>
     <t>STATUS</t>
+  </si>
+  <si>
+    <t>[4/28/2015, 03:58] Pak Devi Leuwigajah: Za yang artesis menu nya belum ada paling di tambahin jumlah pengguna aja klo artesis</t>
+  </si>
+  <si>
+    <t>[4/28/2015, 03:58] Pak Devi Leuwigajah: Blm ada isi nya masih error 404</t>
+  </si>
+  <si>
+    <t>[4/28/2015, 04:01] Pak Devi Leuwigajah: Terus untuk jalan ga usah ada ketersediaan lahan za</t>
+  </si>
+  <si>
+    <t>[4/28/2015, 04:06] Pak Devi Leuwigajah: Dan untuk kategori jalan lebar 1-2m= jalan setapak. 2-4=jalan lingkungan. 4-12= jalan utama</t>
+  </si>
+  <si>
+    <t>[4/28/2015, 04:07] Pak Devi Leuwigajah: Atau untuk ketersediaan lahan untuk jalan isi nya cuma ada atau tidak aja jangan pake angka</t>
+  </si>
+  <si>
+    <t>[4/28/2015, 04:42] Pak Devi Leuwigajah: Za terus untuk posisi koordinat yang longtitude latitude nya di seragamin aja</t>
+  </si>
+  <si>
+    <t>[4/28/2015, 04:43] Pak Devi Leuwigajah: Jadi longtitude awal latitude awal terus longtitude akhir latitude akhir soal na jalan sama drainase beda beda bisi ke lieur entri data na</t>
+  </si>
+  <si>
+    <t>[4/28/2015, 04:59] Pak Devi Leuwigajah: Terus untuk yang "sedang dilaksanakan" kata kata nya di tambah za "sedang / akan dilaksanakan "</t>
   </si>
 </sst>
 </file>
@@ -297,18 +321,6 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -368,6 +380,18 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -384,11 +408,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B78" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
-  <autoFilter ref="A1:B78"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B86" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="3" tableBorderDxfId="4" totalsRowBorderDxfId="2">
+  <autoFilter ref="A1:B86"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="CATATAN" dataDxfId="2"/>
-    <tableColumn id="2" name="STATUS" dataDxfId="1"/>
+    <tableColumn id="1" name="CATATAN" dataDxfId="1"/>
+    <tableColumn id="2" name="STATUS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -681,15 +705,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B78"/>
+  <dimension ref="A1:B86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="146" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="155.7109375" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1124,6 +1148,54 @@
         <v>51</v>
       </c>
       <c r="B78" s="6"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B79" s="2"/>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B80" s="2"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B81" s="2"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B82" s="2"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B83" s="2"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B84" s="2"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B85" s="2"/>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B86" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
perbaikan tampilan menu di data pembangunan membuat access_lib.php untuk menampilkan menu
</commit_message>
<xml_diff>
--- a/DOKUMEN  PENDUKUNG/CATATAN REVISI.xlsx
+++ b/DOKUMEN  PENDUKUNG/CATATAN REVISI.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
   <si>
     <t xml:space="preserve">Print out / Laporan </t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>[4/28/2015, 04:59] Pak Devi Leuwigajah: Terus untuk yang "sedang dilaksanakan" kata kata nya di tambah za "sedang / akan dilaksanakan "</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -361,6 +364,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -368,15 +380,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -408,8 +411,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B86" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="3" tableBorderDxfId="4" totalsRowBorderDxfId="2">
-  <autoFilter ref="A1:B86"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:C86" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
+  <autoFilter ref="B1:C86"/>
   <tableColumns count="2">
     <tableColumn id="1" name="CATATAN" dataDxfId="1"/>
     <tableColumn id="2" name="STATUS" dataDxfId="0"/>
@@ -705,497 +708,500 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B86"/>
+  <dimension ref="A1:C86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="155.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="155.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="2"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="2"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="2"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="2"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="2"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B30" s="2"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="2"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="2"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B33" s="2"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="C33" s="2"/>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="2"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="2"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="C34" s="2"/>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="1"/>
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B36" s="2"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="2"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="2"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="1"/>
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="2"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="2"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="1"/>
+      <c r="C40" s="2"/>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B41" s="2"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="C41" s="2"/>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="2"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="C42" s="2"/>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="2"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="C43" s="2"/>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B44" s="2"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="C44" s="2"/>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="2"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="C45" s="2"/>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B46" s="2"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="C46" s="2"/>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B47" s="2"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+      <c r="C47" s="2"/>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B48" s="2"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="C48" s="2"/>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B49" s="2"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="C49" s="2"/>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B50" s="2"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="2"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="C50" s="2"/>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="1"/>
+      <c r="C51" s="2"/>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B52" s="2"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="2"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+      <c r="C52" s="2"/>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="1"/>
+      <c r="C53" s="2"/>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B54" s="2"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-      <c r="B55" s="2"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+      <c r="C54" s="2"/>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="1"/>
+      <c r="C55" s="2"/>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B56" s="2"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="B57" s="2"/>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+      <c r="C56" s="2"/>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="1"/>
+      <c r="C57" s="2"/>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B58" s="2"/>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="B59" s="2"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-      <c r="B60" s="2"/>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+      <c r="C58" s="2"/>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="1"/>
+      <c r="C59" s="2"/>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="1"/>
+      <c r="C60" s="2"/>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B61" s="2"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="B62" s="2"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+      <c r="C61" s="2"/>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" s="1"/>
+      <c r="C62" s="2"/>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B63" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B63" s="2"/>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
-      <c r="B64" s="2"/>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+      <c r="C63" s="2"/>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B64" s="1"/>
+      <c r="C64" s="2"/>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B65" s="2"/>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-      <c r="B66" s="2"/>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+      <c r="C65" s="2"/>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B66" s="1"/>
+      <c r="C66" s="2"/>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B67" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B67" s="2"/>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
-      <c r="B68" s="2"/>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+      <c r="C67" s="2"/>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B68" s="1"/>
+      <c r="C68" s="2"/>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B69" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B69" s="2"/>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
-      <c r="B70" s="2"/>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+      <c r="C69" s="2"/>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B70" s="1"/>
+      <c r="C70" s="2"/>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B71" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B71" s="2"/>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
-      <c r="B72" s="2"/>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+      <c r="C71" s="2"/>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B72" s="1"/>
+      <c r="C72" s="2"/>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B73" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B73" s="2"/>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
-      <c r="B74" s="2"/>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
+      <c r="C73" s="2"/>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B74" s="1"/>
+      <c r="C74" s="2"/>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B75" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B75" s="2"/>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
-      <c r="B76" s="2"/>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
+      <c r="C75" s="2"/>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B76" s="1"/>
+      <c r="C76" s="2"/>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B77" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B77" s="2"/>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="5" t="s">
+      <c r="C77" s="2"/>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B78" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B78" s="6"/>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
+      <c r="C78" s="6"/>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B79" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B79" s="2"/>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+      <c r="C79" s="2"/>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B80" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B80" s="2"/>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
+      <c r="C80" s="2"/>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B81" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B81" s="2"/>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
+      <c r="C81" s="2"/>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B82" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B82" s="2"/>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
+      <c r="C82" s="2"/>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B83" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B83" s="2"/>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
+      <c r="C83" s="2"/>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B84" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B84" s="2"/>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
+      <c r="C84" s="2"/>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B85" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B85" s="2"/>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="5" t="s">
+      <c r="C85" s="2"/>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B86" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B86" s="6"/>
+      <c r="C86" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
perbaikan bug saat update long ama lat penambahan database/sipepeng_2-5-2015_database_dari_exel.sql
</commit_message>
<xml_diff>
--- a/DOKUMEN  PENDUKUNG/CATATAN REVISI.xlsx
+++ b/DOKUMEN  PENDUKUNG/CATATAN REVISI.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="64">
   <si>
     <t xml:space="preserve">Print out / Laporan </t>
   </si>
@@ -117,9 +117,6 @@
     <t>Laporan</t>
   </si>
   <si>
-    <t>Gt aja pas mau entri di klik icon na</t>
-  </si>
-  <si>
     <t>Terus program kegiatan ga usah paling tupoksi aja gantinya yang dimasukin</t>
   </si>
   <si>
@@ -145,12 +142,6 @@
   </si>
   <si>
     <t>Iya paling warna jalan sama drainase garis na di bedain aja</t>
-  </si>
-  <si>
-    <t>Klo menu jdi icon.. D coba dlu pak..</t>
-  </si>
-  <si>
-    <t>Warna garis.. Nya bsa pak..</t>
   </si>
   <si>
     <t>Terus ukuran garis nya klo jalan rada tebel. drainase rada tipis</t>
@@ -338,7 +329,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -367,56 +378,6 @@
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <border outline="0">
@@ -474,11 +435,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:C88" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="B1:C88"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:C73" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="B1:C73"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="CATATAN" dataDxfId="1"/>
-    <tableColumn id="2" name="STATUS" dataDxfId="0"/>
+    <tableColumn id="1" name="CATATAN" dataDxfId="3"/>
+    <tableColumn id="2" name="STATUS" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -771,10 +732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C88"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,13 +746,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -802,7 +763,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -813,7 +774,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -824,7 +785,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -835,7 +796,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -846,7 +807,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -857,7 +818,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -868,7 +829,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -879,7 +840,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -890,7 +851,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -901,7 +862,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -912,7 +873,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -923,7 +884,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -934,7 +895,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -945,7 +906,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -956,7 +917,7 @@
         <v>13</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -967,7 +928,7 @@
         <v>14</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -978,7 +939,7 @@
         <v>15</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -989,7 +950,7 @@
         <v>16</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1000,7 +961,7 @@
         <v>17</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1011,7 +972,7 @@
         <v>5</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1022,7 +983,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1033,7 +994,7 @@
         <v>5</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1044,7 +1005,7 @@
         <v>19</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1055,7 +1016,7 @@
         <v>20</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1066,7 +1027,7 @@
         <v>21</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1077,7 +1038,7 @@
         <v>22</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1088,638 +1049,495 @@
         <v>23</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" s="1"/>
+        <v>29</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C29" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C32" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>37</v>
-      </c>
-      <c r="B38" s="1"/>
+        <v>42</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="C38" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="B40" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="C40" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>44</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>32</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="B45" s="1"/>
       <c r="C45" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>46</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="B47" s="1"/>
       <c r="C47" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>50</v>
-      </c>
-      <c r="B51" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="C51" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>59</v>
-      </c>
-      <c r="B60" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="C60" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>60</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>42</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="B61" s="1"/>
       <c r="C61" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>61</v>
-      </c>
-      <c r="B62" s="1"/>
+        <v>76</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="C62" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>62</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>43</v>
+        <v>77</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>63</v>
-      </c>
-      <c r="B64" s="1"/>
+        <v>78</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="C64" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>65</v>
-      </c>
-      <c r="B66" s="1"/>
+        <v>80</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="C66" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>67</v>
-      </c>
-      <c r="B68" s="1"/>
+        <v>82</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="C68" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>69</v>
-      </c>
-      <c r="B70" s="1"/>
+        <v>84</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="C70" s="5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>70</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C71" s="5" t="s">
-        <v>64</v>
+        <v>85</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>71</v>
-      </c>
-      <c r="B72" s="1"/>
-      <c r="C72" s="5" t="s">
-        <v>64</v>
+        <v>86</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>72</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>73</v>
-      </c>
-      <c r="B74" s="1"/>
-      <c r="C74" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>74</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C75" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B73" s="4" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>75</v>
-      </c>
-      <c r="B76" s="1"/>
-      <c r="C76" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>76</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C77" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78">
-        <v>77</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C78" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <v>78</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C79" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>79</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C80" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81">
-        <v>80</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C81" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>81</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C82" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83">
-        <v>82</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84">
-        <v>83</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C84" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <v>84</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C85" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <v>85</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C86" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>86</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C87" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88">
-        <v>87</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C88" s="6" t="s">
-        <v>64</v>
+      <c r="C73" s="6" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="ON PROGRESS">
+      <formula>NOT(ISERROR(SEARCH("ON PROGRESS",C1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",C1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="ON PROGRESS">
-      <formula>NOT(ISERROR(SEARCH("ON PROGRESS",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
foto, dokumen berita, update revisian
</commit_message>
<xml_diff>
--- a/DOKUMEN  PENDUKUNG/CATATAN REVISI.xlsx
+++ b/DOKUMEN  PENDUKUNG/CATATAN REVISI.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="78">
   <si>
     <t xml:space="preserve">Print out / Laporan </t>
   </si>
@@ -208,13 +208,58 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beranda tambah berita (berita ada),  gallery, grafik, </t>
+  </si>
+  <si>
+    <t>UMKM tampilkan nama</t>
+  </si>
+  <si>
+    <t>Kontak (isi no kontak)</t>
+  </si>
+  <si>
+    <t>Peta (jalan tambah panjang), satelite (dikecilin  petanya biar muncul satelite)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grafik meliputi : persentase tiap status (usulan, progress, dilaksanakan, tdk dilaksanakan), persentase jumlahnya tiap menu, </t>
+  </si>
+  <si>
+    <t>Hasil print : foto dan dokumen sesuai ukuran sebenarnya, harus bisa langsung cetak tdk edit2 lagi</t>
+  </si>
+  <si>
+    <t>Laporan yg dicetak, tambah logo cimahi (kaya kop surat)</t>
+  </si>
+  <si>
+    <t>umkm (tidak usah dimunculkan kelurahan, kecamatan, kota, bermitra kesana)</t>
+  </si>
+  <si>
+    <t>Jalan 4m jalan utama</t>
+  </si>
+  <si>
+    <t>Sabtu, 25-04-15</t>
+  </si>
+  <si>
+    <t>Sabtu, 02-05-2015</t>
+  </si>
+  <si>
+    <t>foto dalam slide : kuburan kerkof, dll. Jgn sama kaya pa rully</t>
+  </si>
+  <si>
+    <t>menu admin awal iconnya diperkecil, jadi Cuma 1 baris</t>
+  </si>
+  <si>
+    <t xml:space="preserve">berita dari walikota, peresmian </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,13 +267,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="7">
@@ -310,10 +376,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -325,8 +392,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
@@ -435,8 +513,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:C73" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="B1:C73"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:C93" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="B1:C93"/>
   <tableColumns count="2">
     <tableColumn id="1" name="CATATAN" dataDxfId="3"/>
     <tableColumn id="2" name="STATUS" dataDxfId="2"/>
@@ -732,10 +810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:C94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,22 +834,17 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>61</v>
-      </c>
+      <c r="B2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>61</v>
@@ -779,10 +852,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>61</v>
@@ -790,10 +863,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>61</v>
@@ -801,10 +874,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>61</v>
@@ -812,10 +885,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>61</v>
@@ -823,32 +896,32 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>61</v>
@@ -856,10 +929,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>61</v>
@@ -867,10 +940,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>61</v>
@@ -878,10 +951,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>61</v>
@@ -889,10 +962,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>61</v>
@@ -900,10 +973,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>61</v>
@@ -911,10 +984,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>61</v>
@@ -922,10 +995,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>61</v>
@@ -933,10 +1006,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>61</v>
@@ -944,10 +1017,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>61</v>
@@ -955,10 +1028,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>61</v>
@@ -966,10 +1039,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>61</v>
@@ -977,10 +1050,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>61</v>
@@ -988,10 +1061,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>61</v>
@@ -999,21 +1072,21 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>59</v>
@@ -1021,10 +1094,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>59</v>
@@ -1032,21 +1105,21 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>61</v>
@@ -1054,10 +1127,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>61</v>
@@ -1065,43 +1138,43 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C33" s="5" t="s">
         <v>59</v>
@@ -1109,52 +1182,52 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>39</v>
-      </c>
-      <c r="B35" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="C35" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>40</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="B36" s="1"/>
       <c r="C36" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>59</v>
@@ -1162,10 +1235,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>59</v>
@@ -1173,10 +1246,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>59</v>
@@ -1184,10 +1257,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>59</v>
@@ -1195,10 +1268,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>59</v>
@@ -1206,10 +1279,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>59</v>
@@ -1217,61 +1290,61 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>50</v>
-      </c>
-      <c r="B45" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="C45" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>51</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="B46" s="1"/>
       <c r="C46" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>52</v>
-      </c>
-      <c r="B47" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="C47" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>53</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="B48" s="1"/>
       <c r="C48" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>59</v>
@@ -1279,32 +1352,32 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C52" s="5" t="s">
         <v>59</v>
@@ -1312,110 +1385,110 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>67</v>
-      </c>
-      <c r="B53" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="C53" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>68</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>43</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="B54" s="1"/>
       <c r="C54" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>69</v>
-      </c>
-      <c r="B55" s="1"/>
+        <v>68</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="C55" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>70</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>44</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="B56" s="1"/>
       <c r="C56" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>71</v>
-      </c>
-      <c r="B57" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="C57" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>72</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>45</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="B58" s="1"/>
       <c r="C58" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>73</v>
-      </c>
-      <c r="B59" s="1"/>
+        <v>72</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="C59" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>74</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>46</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="B60" s="1"/>
       <c r="C60" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>75</v>
-      </c>
-      <c r="B61" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="C61" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>76</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>47</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="B62" s="1"/>
       <c r="C62" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>77</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>48</v>
+        <v>76</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>61</v>
@@ -1423,10 +1496,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>78</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>51</v>
+        <v>77</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>61</v>
@@ -1434,10 +1507,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>61</v>
@@ -1445,21 +1518,21 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>59</v>
@@ -1467,32 +1540,32 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>59</v>
@@ -1500,36 +1573,203 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>85</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C71" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C71" s="5" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
+        <v>86</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74">
         <v>87</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B74" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C73" s="6" t="s">
-        <v>59</v>
-      </c>
+      <c r="C74" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="11"/>
+      <c r="C75" s="12"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B76" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C76" s="5"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>88</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C77" s="6"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>89</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C78" s="5"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>90</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C79" s="5"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>91</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C80" s="5"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>92</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C81" s="5"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>93</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C82" s="5"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>94</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C83" s="5"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>95</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C84" s="5"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>96</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C85" s="5"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>97</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C86" s="5"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>98</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C87" s="5"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>99</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C88" s="5"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>100</v>
+      </c>
+      <c r="B89" s="4"/>
+      <c r="C89" s="5"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>101</v>
+      </c>
+      <c r="B90" s="4"/>
+      <c r="C90" s="5"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>102</v>
+      </c>
+      <c r="B91" s="4"/>
+      <c r="C91" s="5"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>103</v>
+      </c>
+      <c r="B92" s="4"/>
+      <c r="C92" s="5"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>104</v>
+      </c>
+      <c r="B93" s="4"/>
+      <c r="C93" s="5"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B94" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
@@ -1541,8 +1781,9 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
update CATATAN REVISI.xlsx permohonan KIRMIR  drainase RW.08.doc
</commit_message>
<xml_diff>
--- a/DOKUMEN  PENDUKUNG/CATATAN REVISI.xlsx
+++ b/DOKUMEN  PENDUKUNG/CATATAN REVISI.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="73">
   <si>
     <t xml:space="preserve">Print out / Laporan </t>
   </si>
@@ -90,18 +90,6 @@
     <t xml:space="preserve">Rumah KOS dan Toko : Rekapitulasi per RW </t>
   </si>
   <si>
-    <t>Saat data verifikasi ditolak, harus ada alasannya (1 filed). Diinput manual.</t>
-  </si>
-  <si>
-    <t>Ekonomi dan Pertanian tambah di Menu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diklatpim IV </t>
-  </si>
-  <si>
-    <t>-----------------------------------------------------------</t>
-  </si>
-  <si>
     <t>Ja klo pas nu backproses nya halaman awal na aya nu gini abis login. bisa icon na meh teu langsung masuk</t>
   </si>
   <si>
@@ -153,12 +141,6 @@
     <t>Ada 2 za icon dulu pas di buka icon masuk menu pembangunan</t>
   </si>
   <si>
-    <t>Terus pas di buka icon ekonomi masuk ke economi</t>
-  </si>
-  <si>
-    <t>Terus icon dashboard jg ada</t>
-  </si>
-  <si>
     <t>Surat usulan rw tinggal klik baris data base yang akan di cetak langsung maasuk ka usulan</t>
   </si>
   <si>
@@ -222,9 +204,6 @@
     <t>Peta (jalan tambah panjang), satelite (dikecilin  petanya biar muncul satelite)</t>
   </si>
   <si>
-    <t xml:space="preserve">Grafik meliputi : persentase tiap status (usulan, progress, dilaksanakan, tdk dilaksanakan), persentase jumlahnya tiap menu, </t>
-  </si>
-  <si>
     <t>Hasil print : foto dan dokumen sesuai ukuran sebenarnya, harus bisa langsung cetak tdk edit2 lagi</t>
   </si>
   <si>
@@ -250,6 +229,12 @@
   </si>
   <si>
     <t xml:space="preserve">berita dari walikota, peresmian </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grafik meliputi : persentase tiap status (usulan, progress, dilaksanakan, tdk dilaksanakan), persentase jumlahnya tiap menu (artesis, dll), </t>
+  </si>
+  <si>
+    <t>Revisi cetak surat usulan. Cetak surat dan cetak foto dipisah</t>
   </si>
 </sst>
 </file>
@@ -407,7 +392,27 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -513,11 +518,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:C93" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="B1:C93"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:C81" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="B1:C81"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="CATATAN" dataDxfId="3"/>
-    <tableColumn id="2" name="STATUS" dataDxfId="2"/>
+    <tableColumn id="1" name="CATATAN" dataDxfId="5"/>
+    <tableColumn id="2" name="STATUS" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -810,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C94"/>
+  <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -824,18 +829,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C2" s="8"/>
     </row>
@@ -847,7 +852,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -858,7 +863,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -869,7 +874,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -880,7 +885,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -891,7 +896,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -902,7 +907,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -913,7 +918,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -924,7 +929,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -935,7 +940,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -946,7 +951,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -957,7 +962,7 @@
         <v>10</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -968,7 +973,7 @@
         <v>11</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -979,7 +984,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -990,7 +995,7 @@
         <v>5</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1001,7 +1006,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1012,7 +1017,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1023,7 +1028,7 @@
         <v>15</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1034,7 +1039,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1045,7 +1050,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1056,7 +1061,7 @@
         <v>5</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1067,7 +1072,7 @@
         <v>18</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1078,7 +1083,7 @@
         <v>5</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1089,7 +1094,7 @@
         <v>19</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1100,7 +1105,7 @@
         <v>20</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1111,7 +1116,7 @@
         <v>21</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1122,7 +1127,7 @@
         <v>22</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1133,650 +1138,556 @@
         <v>23</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>39</v>
-      </c>
-      <c r="B36" s="1"/>
+        <v>47</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="C36" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>42</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>30</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="B39" s="1"/>
       <c r="C39" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>44</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>32</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="B41" s="1"/>
       <c r="C41" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>50</v>
-      </c>
-      <c r="B46" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="C46" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>51</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>37</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="B47" s="1"/>
       <c r="C47" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>52</v>
-      </c>
-      <c r="B48" s="1"/>
+        <v>68</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="C48" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>53</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="B49" s="1"/>
       <c r="C49" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>60</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>41</v>
+        <v>77</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>67</v>
-      </c>
-      <c r="B54" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="C54" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>69</v>
-      </c>
-      <c r="B56" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="C56" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>71</v>
-      </c>
-      <c r="B58" s="1"/>
+        <v>83</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="C58" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>73</v>
-      </c>
-      <c r="B60" s="1"/>
-      <c r="C60" s="5" t="s">
-        <v>61</v>
+        <v>85</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>74</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>59</v>
+        <v>86</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>75</v>
-      </c>
-      <c r="B62" s="1"/>
-      <c r="C62" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>76</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>61</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="11"/>
+      <c r="C63" s="12"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>77</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>48</v>
+      <c r="B64" s="7" t="s">
+        <v>67</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>78</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>51</v>
+        <v>88</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>79</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>52</v>
+        <v>89</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>80</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>53</v>
+        <v>90</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>81</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>54</v>
+        <v>91</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>82</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>55</v>
+        <v>92</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>83</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>56</v>
+        <v>93</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>84</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>57</v>
+        <v>94</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C72" s="6" t="s">
-        <v>59</v>
+        <v>64</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C73" s="6" t="s">
-        <v>61</v>
+        <v>65</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C74" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="11"/>
-      <c r="C75" s="12"/>
+        <v>68</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>98</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B76" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C76" s="5"/>
+      <c r="A76">
+        <v>99</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C77" s="6"/>
+        <v>72</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>89</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>65</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="B78" s="4"/>
       <c r="C78" s="5"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>90</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>66</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="B79" s="4"/>
       <c r="C79" s="5"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>91</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>67</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="B80" s="4"/>
       <c r="C80" s="5"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>92</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>68</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="B81" s="4"/>
       <c r="C81" s="5"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>93</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C82" s="5"/>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83">
-        <v>94</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C83" s="5"/>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84">
-        <v>95</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C84" s="5"/>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <v>96</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C85" s="5"/>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86">
-        <v>97</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C86" s="5"/>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87">
-        <v>98</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C87" s="5"/>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88">
-        <v>99</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C88" s="5"/>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89">
-        <v>100</v>
-      </c>
-      <c r="B89" s="4"/>
-      <c r="C89" s="5"/>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90">
-        <v>101</v>
-      </c>
-      <c r="B90" s="4"/>
-      <c r="C90" s="5"/>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91">
-        <v>102</v>
-      </c>
-      <c r="B91" s="4"/>
-      <c r="C91" s="5"/>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <v>103</v>
-      </c>
-      <c r="B92" s="4"/>
-      <c r="C92" s="5"/>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93">
-        <v>104</v>
-      </c>
-      <c r="B93" s="4"/>
-      <c r="C93" s="5"/>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B94" s="9"/>
+      <c r="B82" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="ON PROGRESS">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="ON PROGRESS">
       <formula>NOT(ISERROR(SEARCH("ON PROGRESS",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",C1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
penambahan CATATAN REVISI.xlsx perbaikan ketersediaan_lahan di semua kegiatan perbaikan berita perbaikan slider terbaru perbaikan database/sipepeng_8-5-2015_ubah_database_berita.sql
</commit_message>
<xml_diff>
--- a/DOKUMEN  PENDUKUNG/CATATAN REVISI.xlsx
+++ b/DOKUMEN  PENDUKUNG/CATATAN REVISI.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="93">
   <si>
     <t xml:space="preserve">Print out / Laporan </t>
   </si>
@@ -277,6 +277,24 @@
   </si>
   <si>
     <t>[5/5/2015, 19:40] Pak Devi Leuwigajah: Foto hasil penbangunan jg ada di galeri bawah itu</t>
+  </si>
+  <si>
+    <t>Paling nanti di buat usulan ke pemkot yang di bagian verifikasi berarti item na surat usulan data teknis kaya pajang lebar ketersediaan lahan dll tapi di lembar terpisah. Foto. Dan doc pendukung tea. Tapi jadi na 4 lembar</t>
+  </si>
+  <si>
+    <t>Za klo peta nya ada mode pencarian gt bisa? Jadi ga menampilkan aja yang di bagian public halaman depan</t>
+  </si>
+  <si>
+    <t>Tapi klo buat air bersih sama septictank ada parameter tambahan lupa dari pertama teh. Jumlah pengguna na ga masuk</t>
+  </si>
+  <si>
+    <t>Za punten pang buat keun bisnis proses dari program na dalam bentuk flowchart atau bagan jg boleh cm selembar aja.</t>
+  </si>
+  <si>
+    <t>⁠⁠Ja untuk gambar di web na nu di jadii gambar depan foto pager ini aja za terus yang jembatan pemkot di hapus aja gantinya foto gajah ini</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
@@ -409,27 +427,39 @@
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -437,32 +467,12 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
+        <left/>
+        <right style="thin">
           <color indexed="64"/>
-        </left>
-        <right/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -472,11 +482,12 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
+        <left style="thin">
           <color indexed="64"/>
-        </right>
+        </left>
+        <right/>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -527,6 +538,26 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -541,11 +572,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:C91" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="B1:C91"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:C96" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
+  <autoFilter ref="B1:C96"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="CATATAN" dataDxfId="3"/>
-    <tableColumn id="2" name="STATUS" dataDxfId="2"/>
+    <tableColumn id="1" name="CATATAN" dataDxfId="0"/>
+    <tableColumn id="2" name="STATUS" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -838,10 +869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C92"/>
+  <dimension ref="A1:C96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+    <sheetView tabSelected="1" topLeftCell="B73" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,27 +885,27 @@
       <c r="A1" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="8"/>
+      <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -882,10 +913,10 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -893,10 +924,10 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -904,10 +935,10 @@
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -915,10 +946,10 @@
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -926,10 +957,10 @@
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -937,10 +968,10 @@
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -948,10 +979,10 @@
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -959,10 +990,10 @@
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -970,10 +1001,10 @@
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -981,10 +1012,10 @@
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -992,10 +1023,10 @@
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1003,10 +1034,10 @@
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1014,10 +1045,10 @@
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1025,10 +1056,10 @@
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1036,10 +1067,10 @@
       <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1047,10 +1078,10 @@
       <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1058,10 +1089,10 @@
       <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1069,10 +1100,10 @@
       <c r="A21">
         <v>19</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1080,10 +1111,10 @@
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1091,10 +1122,10 @@
       <c r="A23">
         <v>21</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1102,10 +1133,10 @@
       <c r="A24">
         <v>22</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1113,10 +1144,10 @@
       <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1124,10 +1155,10 @@
       <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1135,10 +1166,10 @@
       <c r="A27">
         <v>25</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1146,10 +1177,10 @@
       <c r="A28">
         <v>26</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1157,10 +1188,10 @@
       <c r="A29">
         <v>27</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1168,10 +1199,10 @@
       <c r="A30">
         <v>40</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1179,10 +1210,10 @@
       <c r="A31">
         <v>41</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1190,10 +1221,10 @@
       <c r="A32">
         <v>42</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1201,10 +1232,10 @@
       <c r="A33">
         <v>43</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1212,10 +1243,10 @@
       <c r="A34">
         <v>44</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1223,10 +1254,10 @@
       <c r="A35">
         <v>46</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1234,10 +1265,10 @@
       <c r="A36">
         <v>47</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1245,10 +1276,10 @@
       <c r="A37">
         <v>48</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1256,10 +1287,10 @@
       <c r="A38">
         <v>49</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1267,8 +1298,8 @@
       <c r="A39">
         <v>50</v>
       </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="5" t="s">
+      <c r="B39" s="10"/>
+      <c r="C39" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1276,10 +1307,10 @@
       <c r="A40">
         <v>51</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1287,8 +1318,8 @@
       <c r="A41">
         <v>52</v>
       </c>
-      <c r="B41" s="1"/>
-      <c r="C41" s="5" t="s">
+      <c r="B41" s="10"/>
+      <c r="C41" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1296,10 +1327,10 @@
       <c r="A42">
         <v>53</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1307,10 +1338,10 @@
       <c r="A43">
         <v>55</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1318,10 +1349,10 @@
       <c r="A44">
         <v>57</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1329,10 +1360,10 @@
       <c r="A45">
         <v>60</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1340,10 +1371,10 @@
       <c r="A46">
         <v>66</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1351,8 +1382,8 @@
       <c r="A47">
         <v>67</v>
       </c>
-      <c r="B47" s="1"/>
-      <c r="C47" s="5" t="s">
+      <c r="B47" s="10"/>
+      <c r="C47" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1360,10 +1391,10 @@
       <c r="A48">
         <v>68</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C48" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1371,8 +1402,8 @@
       <c r="A49">
         <v>69</v>
       </c>
-      <c r="B49" s="1"/>
-      <c r="C49" s="5" t="s">
+      <c r="B49" s="10"/>
+      <c r="C49" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1380,10 +1411,10 @@
       <c r="A50">
         <v>70</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C50" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1391,10 +1422,10 @@
       <c r="A51">
         <v>76</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C51" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1402,10 +1433,10 @@
       <c r="A52">
         <v>77</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C52" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1413,10 +1444,10 @@
       <c r="A53">
         <v>78</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="C53" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1424,10 +1455,10 @@
       <c r="A54">
         <v>79</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="C54" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1435,10 +1466,10 @@
       <c r="A55">
         <v>80</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C55" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1446,10 +1477,10 @@
       <c r="A56">
         <v>81</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="C56" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1457,10 +1488,10 @@
       <c r="A57">
         <v>82</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="C57" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1468,21 +1499,21 @@
       <c r="A58">
         <v>83</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C58" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C58" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>84</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C59" s="3" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1490,10 +1521,10 @@
       <c r="A60">
         <v>85</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="C60" s="4" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1501,10 +1532,10 @@
       <c r="A61">
         <v>86</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C61" s="4" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1512,22 +1543,22 @@
       <c r="A62">
         <v>87</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C62" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="11"/>
-      <c r="C63" s="12"/>
+      <c r="C62" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="12"/>
+      <c r="C63" s="7"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B64" s="7" t="s">
+      <c r="B64" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C64" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1535,10 +1566,10 @@
       <c r="A65">
         <v>88</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C65" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1546,10 +1577,10 @@
       <c r="A66">
         <v>89</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="C66" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1557,10 +1588,10 @@
       <c r="A67">
         <v>90</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C67" s="5" t="s">
+      <c r="C67" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1568,10 +1599,10 @@
       <c r="A68">
         <v>91</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C68" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1579,10 +1610,10 @@
       <c r="A69">
         <v>92</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C69" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1590,10 +1621,10 @@
       <c r="A70">
         <v>93</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C70" s="5" t="s">
+      <c r="C70" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1601,10 +1632,10 @@
       <c r="A71">
         <v>94</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C71" s="5" t="s">
+      <c r="C71" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1612,10 +1643,10 @@
       <c r="A72">
         <v>95</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C72" s="5" t="s">
+      <c r="C72" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1623,10 +1654,10 @@
       <c r="A73">
         <v>96</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B73" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C73" s="5" t="s">
+      <c r="C73" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1634,10 +1665,10 @@
       <c r="A74">
         <v>97</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B74" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C74" s="5" t="s">
+      <c r="C74" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1645,10 +1676,10 @@
       <c r="A75">
         <v>98</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B75" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C75" s="5" t="s">
+      <c r="C75" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1656,10 +1687,10 @@
       <c r="A76">
         <v>99</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B76" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C76" s="5" t="s">
+      <c r="C76" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1667,10 +1698,10 @@
       <c r="A77">
         <v>100</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B77" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="C77" s="3" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1681,134 +1712,178 @@
       <c r="B78" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C78" s="5"/>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C78" s="3"/>
+    </row>
+    <row r="79" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>102</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B79" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C79" s="5"/>
+      <c r="C79" s="3"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>103</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B80" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C80" s="5"/>
+      <c r="C80" s="3"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>104</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B81" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C81" s="5"/>
+      <c r="C81" s="3"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>105</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B82" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C82" s="5"/>
+      <c r="C82" s="3"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>106</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B83" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C83" s="5"/>
+      <c r="C83" s="3"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>107</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B84" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C84" s="5"/>
+      <c r="C84" s="3"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>108</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B85" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C85" s="5"/>
+      <c r="C85" s="3"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>109</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B86" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C86" s="5"/>
+      <c r="C86" s="3"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>110</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B87" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="C87" s="5"/>
+      <c r="C87" s="3"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>111</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B88" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C88" s="5"/>
+      <c r="C88" s="3"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>112</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B89" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C89" s="5"/>
+      <c r="C89" s="3"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>113</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B90" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C90" s="5"/>
+      <c r="C90" s="3"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>114</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B91" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C91" s="5"/>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B92" s="9"/>
+      <c r="C91" s="3"/>
+    </row>
+    <row r="92" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>115</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C92" s="4"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>116</v>
+      </c>
+      <c r="B93" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C93" s="4"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>117</v>
+      </c>
+      <c r="B94" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C94" s="4"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>118</v>
+      </c>
+      <c r="B95" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C95" s="4"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>119</v>
+      </c>
+      <c r="B96" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>92</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="ON PROGRESS">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="ON PROGRESS">
       <formula>NOT(ISERROR(SEARCH("ON PROGRESS",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",C1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update database/sipepeng_10-5-2015_penambahan_field_kontur.sql update CATATAN REVISI.xlsx
</commit_message>
<xml_diff>
--- a/DOKUMEN  PENDUKUNG/CATATAN REVISI.xlsx
+++ b/DOKUMEN  PENDUKUNG/CATATAN REVISI.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="93">
   <si>
     <t xml:space="preserve">Print out / Laporan </t>
   </si>
@@ -27,9 +27,6 @@
     <t>2. Tiap status perencanaan, progress, hasil.</t>
   </si>
   <si>
-    <t xml:space="preserve">3. Surat Usulan (word), Lampiran (foto data awal dan Dokumen pendukung), </t>
-  </si>
-  <si>
     <t>4. Di print ke excel juga</t>
   </si>
   <si>
@@ -295,6 +292,9 @@
   </si>
   <si>
     <t>ok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Surat Usulan (word), Lampiran (detail kegiatan,foto data awal dan Dokumen pendukung), </t>
   </si>
 </sst>
 </file>
@@ -465,14 +465,34 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="10">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
+        <left style="thin">
           <color indexed="64"/>
-        </right>
+        </left>
+        <right/>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -482,12 +502,12 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
+        <left/>
+        <right style="thin">
           <color indexed="64"/>
-        </left>
-        <right/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -572,11 +592,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:C96" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:C96" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="B1:C96"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="CATATAN" dataDxfId="0"/>
-    <tableColumn id="2" name="STATUS" dataDxfId="1"/>
+    <tableColumn id="1" name="CATATAN" dataDxfId="3"/>
+    <tableColumn id="2" name="STATUS" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -871,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B73" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,18 +903,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -906,7 +926,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -917,7 +937,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -928,7 +948,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -936,10 +956,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>3</v>
+        <v>92</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -947,10 +967,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -958,10 +978,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -969,10 +989,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -980,10 +1000,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -991,10 +1011,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1002,10 +1022,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1013,10 +1033,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1024,10 +1044,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1035,10 +1055,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1046,10 +1066,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1057,10 +1077,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1068,10 +1088,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1079,10 +1099,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1090,10 +1110,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1101,10 +1121,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1112,10 +1132,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1123,10 +1143,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1134,10 +1154,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1145,10 +1165,10 @@
         <v>23</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1156,10 +1176,10 @@
         <v>24</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1167,10 +1187,10 @@
         <v>25</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1178,10 +1198,10 @@
         <v>26</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1189,10 +1209,10 @@
         <v>27</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1200,10 +1220,10 @@
         <v>40</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1211,10 +1231,10 @@
         <v>41</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1222,10 +1242,10 @@
         <v>42</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1233,10 +1253,10 @@
         <v>43</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1244,10 +1264,10 @@
         <v>44</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1255,10 +1275,10 @@
         <v>46</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1266,10 +1286,10 @@
         <v>47</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1277,10 +1297,10 @@
         <v>48</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1288,10 +1308,10 @@
         <v>49</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1300,7 +1320,7 @@
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1308,10 +1328,10 @@
         <v>51</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1320,7 +1340,7 @@
       </c>
       <c r="B41" s="10"/>
       <c r="C41" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1328,10 +1348,10 @@
         <v>53</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1339,10 +1359,10 @@
         <v>55</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1350,10 +1370,10 @@
         <v>57</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1361,10 +1381,10 @@
         <v>60</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1372,10 +1392,10 @@
         <v>66</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1384,7 +1404,7 @@
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1392,10 +1412,10 @@
         <v>68</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1404,7 +1424,7 @@
       </c>
       <c r="B49" s="10"/>
       <c r="C49" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1412,10 +1432,10 @@
         <v>70</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1423,10 +1443,10 @@
         <v>76</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1434,10 +1454,10 @@
         <v>77</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1445,10 +1465,10 @@
         <v>78</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1456,10 +1476,10 @@
         <v>79</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1467,10 +1487,10 @@
         <v>80</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1478,10 +1498,10 @@
         <v>81</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1489,10 +1509,10 @@
         <v>82</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1500,10 +1520,10 @@
         <v>83</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1511,10 +1531,10 @@
         <v>84</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1522,10 +1542,10 @@
         <v>85</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1533,10 +1553,10 @@
         <v>86</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -1544,10 +1564,10 @@
         <v>87</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="63" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1556,10 +1576,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B64" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1567,10 +1587,10 @@
         <v>88</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1578,10 +1598,10 @@
         <v>89</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1589,10 +1609,10 @@
         <v>90</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -1600,10 +1620,10 @@
         <v>91</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1611,10 +1631,10 @@
         <v>92</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -1622,10 +1642,10 @@
         <v>93</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -1633,10 +1653,10 @@
         <v>94</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -1644,10 +1664,10 @@
         <v>95</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -1655,10 +1675,10 @@
         <v>96</v>
       </c>
       <c r="B73" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -1666,10 +1686,10 @@
         <v>97</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -1677,10 +1697,10 @@
         <v>98</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -1688,10 +1708,10 @@
         <v>99</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -1699,10 +1719,10 @@
         <v>100</v>
       </c>
       <c r="B77" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -1710,180 +1730,216 @@
         <v>101</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="C78" s="3"/>
+        <v>72</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="79" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>102</v>
       </c>
       <c r="B79" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="C79" s="3"/>
+        <v>73</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>103</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="C80" s="3"/>
+        <v>74</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>104</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C81" s="3"/>
+        <v>75</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>105</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C82" s="3"/>
+        <v>76</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>106</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="C83" s="3"/>
+        <v>77</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>107</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C84" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>108</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C85" s="3"/>
+        <v>79</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>109</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C86" s="3"/>
+        <v>80</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>110</v>
       </c>
       <c r="B87" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C87" s="3"/>
+        <v>81</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>111</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C88" s="3"/>
+        <v>82</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>112</v>
       </c>
       <c r="B89" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C89" s="3"/>
+        <v>83</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>113</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C90" s="3"/>
+        <v>84</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>114</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="C91" s="3"/>
+        <v>85</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="92" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>115</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="C92" s="4"/>
+        <v>86</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>116</v>
       </c>
       <c r="B93" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="C93" s="4"/>
+        <v>87</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>117</v>
       </c>
       <c r="B94" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="C94" s="4"/>
+        <v>88</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>118</v>
       </c>
       <c r="B95" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="C95" s="4"/>
+        <v>89</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>119</v>
       </c>
       <c r="B96" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C96" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="C96" s="4" t="s">
-        <v>92</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="ON PROGRESS">
+    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="ON PROGRESS">
       <formula>NOT(ISERROR(SEARCH("ON PROGRESS",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",C1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
perbaikan menu hasil pembangunan perbaikan menu di home admin/home.php perbaikan artesis dan septictank -> penambahan jumlah pengguna perbaikan CATATAN REVISI.xlsx
</commit_message>
<xml_diff>
--- a/DOKUMEN  PENDUKUNG/CATATAN REVISI.xlsx
+++ b/DOKUMEN  PENDUKUNG/CATATAN REVISI.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="92">
   <si>
     <t xml:space="preserve">Print out / Laporan </t>
   </si>
@@ -25,9 +25,6 @@
   </si>
   <si>
     <t>2. Tiap status perencanaan, progress, hasil.</t>
-  </si>
-  <si>
-    <t>4. Di print ke excel juga</t>
   </si>
   <si>
     <t>--</t>
@@ -465,7 +462,7 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -558,26 +555,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -592,8 +569,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:C96" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="B1:C96"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:C91" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+  <autoFilter ref="B1:C91"/>
   <tableColumns count="2">
     <tableColumn id="1" name="CATATAN" dataDxfId="3"/>
     <tableColumn id="2" name="STATUS" dataDxfId="2"/>
@@ -889,10 +866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C96"/>
+  <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,18 +880,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -926,7 +903,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -937,7 +914,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -948,7 +925,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -956,990 +933,943 @@
         <v>4</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B30" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B31" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B32" s="10" t="s">
         <v>25</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>26</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B34" s="10" t="s">
         <v>27</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B35" s="10" t="s">
         <v>28</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B36" s="10" t="s">
         <v>29</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B37" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B38" s="10" t="s">
         <v>31</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>50</v>
-      </c>
-      <c r="B39" s="10"/>
+        <v>53</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="C39" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>52</v>
-      </c>
-      <c r="B41" s="10"/>
+        <v>57</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>34</v>
+      </c>
       <c r="C41" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>67</v>
-      </c>
-      <c r="B47" s="10"/>
+        <v>77</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="C47" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>69</v>
-      </c>
-      <c r="B49" s="10"/>
+        <v>79</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>44</v>
+      </c>
       <c r="C49" s="3" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>77</v>
-      </c>
-      <c r="B52" s="11" t="s">
-        <v>41</v>
+        <v>82</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>80</v>
-      </c>
-      <c r="B55" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>52</v>
+        <v>85</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>81</v>
-      </c>
-      <c r="B56" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C56" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B56" s="11" t="s">
         <v>52</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>82</v>
-      </c>
-      <c r="B57" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C57" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B57" s="11" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>83</v>
-      </c>
-      <c r="B58" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>84</v>
-      </c>
-      <c r="B59" s="10" t="s">
-        <v>50</v>
+      <c r="C57" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="12"/>
+      <c r="C58" s="7"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="9" t="s">
+        <v>65</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>52</v>
+        <v>56</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>52</v>
+        <v>57</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="12"/>
-      <c r="C63" s="7"/>
+        <v>58</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>91</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B64" s="9" t="s">
-        <v>66</v>
+      <c r="A64">
+        <v>92</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>69</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>96</v>
-      </c>
-      <c r="B73" s="11" t="s">
-        <v>64</v>
+        <v>101</v>
+      </c>
+      <c r="B73" s="13" t="s">
+        <v>71</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>100</v>
-      </c>
-      <c r="B77" s="11" t="s">
-        <v>71</v>
+        <v>105</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>101</v>
-      </c>
-      <c r="B78" s="13" t="s">
-        <v>72</v>
+        <v>106</v>
+      </c>
+      <c r="B78" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>102</v>
-      </c>
-      <c r="B79" s="11" t="s">
-        <v>73</v>
+        <v>107</v>
+      </c>
+      <c r="B79" s="10" t="s">
+        <v>77</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>103</v>
-      </c>
-      <c r="B80" s="11" t="s">
-        <v>74</v>
+        <v>108</v>
+      </c>
+      <c r="B80" s="10" t="s">
+        <v>78</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>104</v>
-      </c>
-      <c r="B81" s="11" t="s">
-        <v>75</v>
+        <v>109</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>79</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>91</v>
+        <v>53</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>110</v>
-      </c>
-      <c r="B87" s="10" t="s">
-        <v>81</v>
+        <v>115</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>111</v>
-      </c>
-      <c r="B88" s="10" t="s">
-        <v>82</v>
+        <v>116</v>
+      </c>
+      <c r="B88" s="11" t="s">
+        <v>86</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>112</v>
-      </c>
-      <c r="B89" s="10" t="s">
-        <v>83</v>
+        <v>117</v>
+      </c>
+      <c r="B89" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>113</v>
-      </c>
-      <c r="B90" s="10" t="s">
-        <v>84</v>
+        <v>118</v>
+      </c>
+      <c r="B90" s="11" t="s">
+        <v>88</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>114</v>
-      </c>
-      <c r="B91" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C91" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A92">
-        <v>115</v>
-      </c>
-      <c r="B92" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C92" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93">
-        <v>116</v>
-      </c>
-      <c r="B93" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94">
-        <v>117</v>
-      </c>
-      <c r="B94" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95">
-        <v>118</v>
-      </c>
-      <c r="B95" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B91" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="C95" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96">
-        <v>119</v>
-      </c>
-      <c r="B96" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="C96" s="4" t="s">
-        <v>91</v>
+      <c r="C91" s="4" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="ON PROGRESS">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="ON PROGRESS">
       <formula>NOT(ISERROR(SEARCH("ON PROGRESS",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",C1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
cetak keseluruhan penambahan CATATAN REVISI.xlsx perbaikan tampilan
</commit_message>
<xml_diff>
--- a/DOKUMEN  PENDUKUNG/CATATAN REVISI.xlsx
+++ b/DOKUMEN  PENDUKUNG/CATATAN REVISI.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="98">
   <si>
     <t xml:space="preserve">Print out / Laporan </t>
   </si>
@@ -292,6 +292,24 @@
   </si>
   <si>
     <t xml:space="preserve">3. Surat Usulan (word), Lampiran (detail kegiatan,foto data awal dan Dokumen pendukung), </t>
+  </si>
+  <si>
+    <t>[5/13/2015, 00:41] Pak Devi Leuwigajah: Za barusan udah dikirim data yang hasil pembangunan sama yang akan di bangun 2015. Cobain aja dulu tar klo ada yanh aneh peta nya kasi tau</t>
+  </si>
+  <si>
+    <t>[5/13/2015, 00:42] Pak Devi Leuwigajah: Itu kelemahan peta nya klo ada belokan susah jadi cuma bisa lurus aja</t>
+  </si>
+  <si>
+    <t>[5/13/2015, 00:42] Pak Devi Leuwigajah: Untuk jalan sama drainase</t>
+  </si>
+  <si>
+    <t>[5/13/2015, 18:09] Pak Devi Leuwigajah: Za gimana kemaren udah bisa di masukin data base yang di email nya?</t>
+  </si>
+  <si>
+    <t>[5/13/2015, 18:09] Pak Devi Leuwigajah: Ada yang aneh ga koordinat nya</t>
+  </si>
+  <si>
+    <t>Terus za ini data usulan dah mulai ada. Yang di masukinnya nanti di exel berdasrkan kegiatan aja jadi dari rw.01 sampe 20</t>
   </si>
 </sst>
 </file>
@@ -464,26 +482,6 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -555,6 +553,26 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -569,11 +587,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:C91" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
-  <autoFilter ref="B1:C91"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:C97" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
+  <autoFilter ref="B1:C97"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="CATATAN" dataDxfId="3"/>
-    <tableColumn id="2" name="STATUS" dataDxfId="2"/>
+    <tableColumn id="1" name="CATATAN" dataDxfId="1"/>
+    <tableColumn id="2" name="STATUS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -866,10 +884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C91"/>
+  <dimension ref="A1:C97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1864,12 +1882,48 @@
         <v>90</v>
       </c>
     </row>
+    <row r="92" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B92" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C92" s="3"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B93" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C93" s="3"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B94" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C94" s="3"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B95" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C95" s="3"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B96" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C96" s="4"/>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B97" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C97" s="4"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="ON PROGRESS">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="ON PROGRESS">
       <formula>NOT(ISERROR(SEARCH("ON PROGRESS",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",C1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update slider/leuwigajah.jpg update ukuran slider update drainase_managements.php
</commit_message>
<xml_diff>
--- a/DOKUMEN  PENDUKUNG/CATATAN REVISI.xlsx
+++ b/DOKUMEN  PENDUKUNG/CATATAN REVISI.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="106">
   <si>
     <t xml:space="preserve">Print out / Laporan </t>
   </si>
@@ -506,26 +506,6 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -597,6 +577,26 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -611,11 +611,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:C126" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:C126" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
   <autoFilter ref="B1:C126"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="CATATAN" dataDxfId="3"/>
-    <tableColumn id="2" name="STATUS" dataDxfId="2"/>
+    <tableColumn id="1" name="CATATAN" dataDxfId="1"/>
+    <tableColumn id="2" name="STATUS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -911,7 +911,7 @@
   <dimension ref="A1:C126"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99"/>
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1940,7 +1940,9 @@
       <c r="B95" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C95" s="3"/>
+      <c r="C95" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
@@ -2115,10 +2117,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="ON PROGRESS">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="ON PROGRESS">
       <formula>NOT(ISERROR(SEARCH("ON PROGRESS",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",C1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update CATATAN REVISI.xlsx dan data baru dari pa devi
</commit_message>
<xml_diff>
--- a/DOKUMEN  PENDUKUNG/CATATAN REVISI.xlsx
+++ b/DOKUMEN  PENDUKUNG/CATATAN REVISI.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="112">
   <si>
     <t xml:space="preserve">Print out / Laporan </t>
   </si>
@@ -334,6 +334,24 @@
   </si>
   <si>
     <t>Kata-kata di slide, ubah jadi berita</t>
+  </si>
+  <si>
+    <t>bisa cetak surat usulan, file rincian kegiatan (semua)</t>
+  </si>
+  <si>
+    <t>di umkm: ditampilkan nama, hapus kelurahan, kecamatan, kota</t>
+  </si>
+  <si>
+    <t>gallery di link sama hasil2 pembangunan</t>
+  </si>
+  <si>
+    <t>perbaikan bug foto dan dokumen</t>
+  </si>
+  <si>
+    <t>database di hapus, diganti dengan data2 yang baru</t>
+  </si>
+  <si>
+    <t>kata-kata di bawah blog di hapus</t>
   </si>
 </sst>
 </file>
@@ -910,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="C96" sqref="C96"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2033,31 +2051,64 @@
       <c r="B106" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C106" s="3"/>
+      <c r="C106" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B107" s="11"/>
+      <c r="A107">
+        <v>135</v>
+      </c>
+      <c r="B107" s="11" t="s">
+        <v>106</v>
+      </c>
       <c r="C107" s="3"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B108" s="11"/>
-      <c r="C108" s="3"/>
+      <c r="A108">
+        <v>136</v>
+      </c>
+      <c r="B108" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B109" s="11"/>
+      <c r="A109">
+        <v>137</v>
+      </c>
+      <c r="B109" s="11" t="s">
+        <v>108</v>
+      </c>
       <c r="C109" s="3"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B110" s="11"/>
+      <c r="A110">
+        <v>138</v>
+      </c>
+      <c r="B110" s="11" t="s">
+        <v>109</v>
+      </c>
       <c r="C110" s="3"/>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B111" s="11"/>
+      <c r="A111">
+        <v>139</v>
+      </c>
+      <c r="B111" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="C111" s="3"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B112" s="11"/>
-      <c r="C112" s="3"/>
+      <c r="B112" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" s="11"/>

</xml_diff>

<commit_message>
fix foto drainase fix database foto drainase ubah font Manual Book.docx
</commit_message>
<xml_diff>
--- a/DOKUMEN  PENDUKUNG/CATATAN REVISI.xlsx
+++ b/DOKUMEN  PENDUKUNG/CATATAN REVISI.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="137">
   <si>
     <t xml:space="preserve">Print out / Laporan </t>
   </si>
@@ -424,6 +424,9 @@
   </si>
   <si>
     <t>[5/25/2015, 17:13] Pak Devi Leuwigajah: Sekarang dikirim lagi foto yang drainase yg sedan/ akan dilaksanakan</t>
+  </si>
+  <si>
+    <t>not</t>
   </si>
 </sst>
 </file>
@@ -596,26 +599,6 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -687,6 +670,26 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -701,11 +704,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:C136" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B1:C136" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
   <autoFilter ref="B1:C136"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="CATATAN" dataDxfId="3"/>
-    <tableColumn id="2" name="STATUS" dataDxfId="2"/>
+    <tableColumn id="1" name="CATATAN" dataDxfId="1"/>
+    <tableColumn id="2" name="STATUS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1000,8 +1003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="B113" sqref="B113:B136"/>
+    <sheetView tabSelected="1" topLeftCell="B101" workbookViewId="0">
+      <selection activeCell="C137" sqref="C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2069,7 +2072,9 @@
       <c r="B100" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C100" s="3"/>
+      <c r="C100" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
@@ -2078,7 +2083,9 @@
       <c r="B101" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="C101" s="3"/>
+      <c r="C101" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
@@ -2087,7 +2094,9 @@
       <c r="B102" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="C102" s="3"/>
+      <c r="C102" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103">
@@ -2096,7 +2105,9 @@
       <c r="B103" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="C103" s="3"/>
+      <c r="C103" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104">
@@ -2105,7 +2116,9 @@
       <c r="B104" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C104" s="3"/>
+      <c r="C104" s="3" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
@@ -2114,7 +2127,9 @@
       <c r="B105" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C105" s="3"/>
+      <c r="C105" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106">
@@ -2134,7 +2149,9 @@
       <c r="B107" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="C107" s="3"/>
+      <c r="C107" s="3" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108">
@@ -2154,7 +2171,9 @@
       <c r="B109" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="C109" s="3"/>
+      <c r="C109" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
@@ -2172,7 +2191,9 @@
       <c r="B111" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="C111" s="3"/>
+      <c r="C111" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B112" s="11" t="s">
@@ -2186,152 +2207,200 @@
       <c r="B113" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="C113" s="3"/>
+      <c r="C113" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="C114" s="3"/>
+      <c r="C114" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="C115" s="3"/>
+      <c r="C115" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="C116" s="3"/>
+      <c r="C116" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="C117" s="3"/>
+      <c r="C117" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="C118" s="3"/>
+      <c r="C118" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="C119" s="3"/>
+      <c r="C119" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="C120" s="3"/>
+      <c r="C120" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="C121" s="3"/>
+      <c r="C121" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B122" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="C122" s="3"/>
+      <c r="C122" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B123" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="C123" s="3"/>
+      <c r="C123" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B124" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="C124" s="3"/>
+      <c r="C124" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B125" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="C125" s="3"/>
+      <c r="C125" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B126" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="C126" s="3"/>
+      <c r="C126" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B127" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="C127" s="3"/>
+      <c r="C127" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B128" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="C128" s="3"/>
+      <c r="C128" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="C129" s="3"/>
+      <c r="C129" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="C130" s="3"/>
+      <c r="C130" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="C131" s="3"/>
+      <c r="C131" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="C132" s="3"/>
+      <c r="C132" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="C133" s="3"/>
+      <c r="C133" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C134" s="3"/>
+      <c r="C134" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B135" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="C135" s="3"/>
+      <c r="C135" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="C136" s="3"/>
+      <c r="C136" s="3" t="s">
+        <v>90</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="ON PROGRESS">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="ON PROGRESS">
       <formula>NOT(ISERROR(SEARCH("ON PROGRESS",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="OK">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="OK">
       <formula>NOT(ISERROR(SEARCH("OK",C1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>